<commit_message>
Latest code snapshot from the archive
- VB.NET version
- GameMaker DLL
- A bunch of other changes I don't remember
</commit_message>
<xml_diff>
--- a/doc/Frequency Range.xlsx
+++ b/doc/Frequency Range.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="213">
   <si>
     <t>a</t>
   </si>
@@ -309,349 +309,352 @@
     <t>B3</t>
   </si>
   <si>
+    <t>n - 52 (&amp;a)</t>
+  </si>
+  <si>
+    <t>F#1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>D#1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C#1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>A#0</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>G#0</t>
+  </si>
+  <si>
+    <t>G0</t>
+  </si>
+  <si>
+    <t>F#0</t>
+  </si>
+  <si>
+    <t>F0</t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>D#0</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>C#0</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>B-1</t>
+  </si>
+  <si>
+    <t>A#-1</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>G#-1</t>
+  </si>
+  <si>
+    <t>G-1</t>
+  </si>
+  <si>
+    <t>F#-1</t>
+  </si>
+  <si>
+    <t>F-1</t>
+  </si>
+  <si>
+    <t>E-1</t>
+  </si>
+  <si>
+    <t>D#-1</t>
+  </si>
+  <si>
+    <t>D-1</t>
+  </si>
+  <si>
+    <t>C#-1</t>
+  </si>
+  <si>
+    <t>C-1</t>
+  </si>
+  <si>
+    <t>B-2</t>
+  </si>
+  <si>
+    <t>A#-2</t>
+  </si>
+  <si>
+    <t>A-2</t>
+  </si>
+  <si>
+    <t>G#-2</t>
+  </si>
+  <si>
+    <t>G-2</t>
+  </si>
+  <si>
+    <t>F#-2</t>
+  </si>
+  <si>
+    <t>F-2</t>
+  </si>
+  <si>
+    <t>E-2</t>
+  </si>
+  <si>
+    <t>D#-2</t>
+  </si>
+  <si>
+    <t>n +50 (&amp;Z)</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C#7</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D#7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F#7</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G#7</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A#7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C#8</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D#8</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F#8</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G#8</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>A#8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C#9</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D#9</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F#9</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G#9</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>A#9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C#10</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D#10</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F#10</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G#10</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A#10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>Basic range</t>
+  </si>
+  <si>
+    <t>Lowest range</t>
+  </si>
+  <si>
+    <t>Highest range</t>
+  </si>
+  <si>
+    <t>G#4</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>F#4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>D#4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>C#4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>G#3</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>F#3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>D#3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>C#3</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
-    <t>C#3</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D#3</t>
-  </si>
-  <si>
-    <t>E3</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F#3</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G#3</t>
-  </si>
-  <si>
-    <t>n - 52 (&amp;a)</t>
-  </si>
-  <si>
-    <t>F#1</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>D#1</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>C#1</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>B0</t>
-  </si>
-  <si>
-    <t>A#0</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>G#0</t>
-  </si>
-  <si>
-    <t>G0</t>
-  </si>
-  <si>
-    <t>F#0</t>
-  </si>
-  <si>
-    <t>F0</t>
-  </si>
-  <si>
-    <t>E0</t>
-  </si>
-  <si>
-    <t>D#0</t>
-  </si>
-  <si>
-    <t>D0</t>
-  </si>
-  <si>
-    <t>C#0</t>
-  </si>
-  <si>
-    <t>C0</t>
-  </si>
-  <si>
-    <t>B-1</t>
-  </si>
-  <si>
-    <t>A#-1</t>
-  </si>
-  <si>
-    <t>A-1</t>
-  </si>
-  <si>
-    <t>G#-1</t>
-  </si>
-  <si>
-    <t>G-1</t>
-  </si>
-  <si>
-    <t>F#-1</t>
-  </si>
-  <si>
-    <t>F-1</t>
-  </si>
-  <si>
-    <t>E-1</t>
-  </si>
-  <si>
-    <t>D#-1</t>
-  </si>
-  <si>
-    <t>D-1</t>
-  </si>
-  <si>
-    <t>C#-1</t>
-  </si>
-  <si>
-    <t>C-1</t>
-  </si>
-  <si>
-    <t>B-2</t>
-  </si>
-  <si>
-    <t>A#-2</t>
-  </si>
-  <si>
-    <t>A-2</t>
-  </si>
-  <si>
-    <t>G#-2</t>
-  </si>
-  <si>
-    <t>G-2</t>
-  </si>
-  <si>
-    <t>F#-2</t>
-  </si>
-  <si>
-    <t>F-2</t>
-  </si>
-  <si>
-    <t>E-2</t>
-  </si>
-  <si>
-    <t>D#-2</t>
-  </si>
-  <si>
-    <t>D-2</t>
-  </si>
-  <si>
-    <t>C#-2</t>
-  </si>
-  <si>
-    <t>C-2</t>
-  </si>
-  <si>
-    <t>B-3</t>
-  </si>
-  <si>
-    <t>A#-3</t>
-  </si>
-  <si>
-    <t>A-3</t>
-  </si>
-  <si>
-    <t>G#-3</t>
-  </si>
-  <si>
-    <t>G-3</t>
-  </si>
-  <si>
-    <t>F#-3</t>
-  </si>
-  <si>
-    <t>F-3</t>
-  </si>
-  <si>
-    <t>E-3</t>
-  </si>
-  <si>
-    <t>D#-3</t>
-  </si>
-  <si>
-    <t>n +50 (&amp;Z)</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C#7</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D#7</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>F#7</t>
-  </si>
-  <si>
-    <t>G7</t>
-  </si>
-  <si>
-    <t>G#7</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A#7</t>
-  </si>
-  <si>
-    <t>B8</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C#8</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>D#8</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>F#8</t>
-  </si>
-  <si>
-    <t>G8</t>
-  </si>
-  <si>
-    <t>G#8</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A#8</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C#9</t>
-  </si>
-  <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>D#9</t>
-  </si>
-  <si>
-    <t>E9</t>
-  </si>
-  <si>
-    <t>F9</t>
-  </si>
-  <si>
-    <t>F#9</t>
-  </si>
-  <si>
-    <t>G9</t>
-  </si>
-  <si>
-    <t>G#9</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A#9</t>
-  </si>
-  <si>
-    <t>B10</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C#10</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>D#10</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
-    <t>F#10</t>
-  </si>
-  <si>
-    <t>G10</t>
-  </si>
-  <si>
-    <t>G#10</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A#10</t>
-  </si>
-  <si>
-    <t>B11</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>Basic range</t>
-  </si>
-  <si>
-    <t>Lowest range</t>
-  </si>
-  <si>
-    <t>Highest range</t>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A#1</t>
+  </si>
+  <si>
+    <t>B1</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O55"/>
+  <dimension ref="B2:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I38" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,21 +1065,21 @@
   <sheetData>
     <row r="2" spans="2:15" ht="33.75" x14ac:dyDescent="0.5">
       <c r="B2" s="6" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="2"/>
       <c r="G2" s="6" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="2"/>
       <c r="L2" s="6" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -1100,7 +1103,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>10</v>
@@ -1113,7 +1116,7 @@
         <v>52</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>10</v>
@@ -1134,7 +1137,7 @@
         <v>97.998858995437345</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>0</v>
@@ -1148,7 +1151,7 @@
         <v>4.5885119987094942</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>0</v>
@@ -1177,7 +1180,7 @@
         <v>103.82617439498628</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>1</v>
@@ -1191,13 +1194,13 @@
         <v>5.1504305767635916</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" ref="M5:M55" si="3">C5+50</f>
+        <f t="shared" ref="M5:M54" si="3">C5+50</f>
         <v>25</v>
       </c>
       <c r="N5" s="4">
@@ -1234,7 +1237,7 @@
         <v>5.4566911161406892</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>2</v>
@@ -1248,7 +1251,7 @@
         <v>1975.5332050244961</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1277,7 +1280,7 @@
         <v>5.7811628548692866</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>3</v>
@@ -1291,7 +1294,7 @@
         <v>2093.004522404789</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -1320,7 +1323,7 @@
         <v>6.1249286872148323</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>4</v>
@@ -1334,7 +1337,7 @@
         <v>2217.4610478149771</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -1349,7 +1352,7 @@
         <v>130.81278265029931</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>208</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>5</v>
@@ -1363,7 +1366,7 @@
         <v>6.4891358996866435</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>5</v>
@@ -1377,7 +1380,7 @@
         <v>2349.3181433392601</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -1392,7 +1395,7 @@
         <v>138.59131548843604</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>207</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>6</v>
@@ -1406,7 +1409,7 @@
         <v>6.875</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>6</v>
@@ -1420,7 +1423,7 @@
         <v>2489.0158697766474</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -1435,7 +1438,7 @@
         <v>146.83238395870382</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>7</v>
@@ -1449,7 +1452,7 @@
         <v>7.2838087737201525</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>7</v>
@@ -1463,7 +1466,7 @@
         <v>2637.0204553029598</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -1478,7 +1481,7 @@
         <v>155.56349186104046</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>89</v>
+        <v>205</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
@@ -1492,7 +1495,7 @@
         <v>7.7169265821269439</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>8</v>
@@ -1506,7 +1509,7 @@
         <v>2793.8258514640311</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1521,7 +1524,7 @@
         <v>164.81377845643496</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>90</v>
+        <v>204</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>9</v>
@@ -1535,7 +1538,7 @@
         <v>8.175798915643707</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>9</v>
@@ -1549,7 +1552,7 @@
         <v>2959.9553816930757</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -1564,7 +1567,7 @@
         <v>174.61411571650197</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>91</v>
+        <v>203</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>10</v>
@@ -1578,7 +1581,7 @@
         <v>8.6619572180272524</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>10</v>
@@ -1592,7 +1595,7 @@
         <v>3135.9634878539941</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -1607,7 +1610,7 @@
         <v>184.99721135581723</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>11</v>
@@ -1621,7 +1624,7 @@
         <v>9.1770239974189884</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>11</v>
@@ -1635,7 +1638,7 @@
         <v>3322.4375806395601</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -1650,7 +1653,7 @@
         <v>195.99771799087463</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>12</v>
@@ -1664,7 +1667,7 @@
         <v>9.722718241315027</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>12</v>
@@ -1678,7 +1681,7 @@
         <v>3520</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -1693,7 +1696,7 @@
         <v>207.65234878997259</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>13</v>
@@ -1707,7 +1710,7 @@
         <v>10.300861153527187</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>13</v>
@@ -1721,7 +1724,7 @@
         <v>3729.3100921447194</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -1750,7 +1753,7 @@
         <v>10.913382232281375</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>14</v>
@@ -1764,7 +1767,7 @@
         <v>3951.0664100489917</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -1793,7 +1796,7 @@
         <v>11.562325709738577</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
@@ -1807,7 +1810,7 @@
         <v>4186.0090448095771</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -1836,7 +1839,7 @@
         <v>12.249857374429663</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>16</v>
@@ -1850,7 +1853,7 @@
         <v>4434.9220956299532</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -1865,7 +1868,7 @@
         <v>261.62556530059862</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>17</v>
@@ -1879,7 +1882,7 @@
         <v>12.978271799373291</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>17</v>
@@ -1893,7 +1896,7 @@
         <v>4698.6362866785194</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -1908,7 +1911,7 @@
         <v>277.18263097687208</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>18</v>
@@ -1922,7 +1925,7 @@
         <v>13.75</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>18</v>
@@ -1936,7 +1939,7 @@
         <v>4978.0317395532938</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -1951,7 +1954,7 @@
         <v>293.66476791740757</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>19</v>
@@ -1965,7 +1968,7 @@
         <v>14.567617547440307</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>19</v>
@@ -1979,7 +1982,7 @@
         <v>5274.0409106059187</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -1994,7 +1997,7 @@
         <v>311.12698372208087</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>100</v>
+        <v>196</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>20</v>
@@ -2008,7 +2011,7 @@
         <v>15.433853164253883</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>20</v>
@@ -2022,7 +2025,7 @@
         <v>5587.6517029280612</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -2037,7 +2040,7 @@
         <v>329.62755691286992</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>101</v>
+        <v>195</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>21</v>
@@ -2051,7 +2054,7 @@
         <v>16.351597831287414</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>21</v>
@@ -2065,7 +2068,7 @@
         <v>5919.9107633861504</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -2080,7 +2083,7 @@
         <v>349.22823143300388</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>102</v>
+        <v>194</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>22</v>
@@ -2094,7 +2097,7 @@
         <v>17.323914436054505</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>22</v>
@@ -2108,7 +2111,7 @@
         <v>6271.9269757079892</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -2123,7 +2126,7 @@
         <v>369.99442271163446</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
+        <v>193</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>23</v>
@@ -2137,7 +2140,7 @@
         <v>18.354047994837977</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>23</v>
@@ -2151,7 +2154,7 @@
         <v>6644.8751612791211</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
@@ -2166,7 +2169,7 @@
         <v>391.99543598174927</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>104</v>
+        <v>192</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>24</v>
@@ -2180,7 +2183,7 @@
         <v>19.445436482630058</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>24</v>
@@ -2194,7 +2197,7 @@
         <v>7040</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -2209,7 +2212,7 @@
         <v>415.30469757994513</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>25</v>
@@ -2223,7 +2226,7 @@
         <v>20.601722307054366</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="L29" s="3" t="s">
         <v>25</v>
@@ -2237,7 +2240,7 @@
         <v>7458.6201842894361</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -2266,7 +2269,7 @@
         <v>21.82676446456275</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>26</v>
@@ -2280,7 +2283,7 @@
         <v>7902.1328200979879</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
@@ -2309,7 +2312,7 @@
         <v>23.124651419477154</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>27</v>
@@ -2323,7 +2326,7 @@
         <v>8372.0180896191559</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
@@ -2352,7 +2355,7 @@
         <v>24.499714748859326</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>28</v>
@@ -2366,7 +2369,7 @@
         <v>8869.8441912599046</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
@@ -2395,7 +2398,7 @@
         <v>25.956543598746581</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="L33" s="3" t="s">
         <v>29</v>
@@ -2409,7 +2412,7 @@
         <v>9397.2725733570442</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
@@ -2438,7 +2441,7 @@
         <v>27.5</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="L34" s="3" t="s">
         <v>30</v>
@@ -2452,7 +2455,7 @@
         <v>9956.0634791065877</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
@@ -2481,7 +2484,7 @@
         <v>29.135235094880628</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>31</v>
@@ -2495,7 +2498,7 @@
         <v>10548.081821211836</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
@@ -2524,7 +2527,7 @@
         <v>30.867706328507751</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="L36" s="3" t="s">
         <v>32</v>
@@ -2538,7 +2541,7 @@
         <v>11175.303405856126</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
@@ -2567,7 +2570,7 @@
         <v>32.703195662574828</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>33</v>
@@ -2581,7 +2584,7 @@
         <v>11839.821526772301</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
@@ -2610,7 +2613,7 @@
         <v>34.647828872109017</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="L38" s="3" t="s">
         <v>34</v>
@@ -2624,7 +2627,7 @@
         <v>12543.853951415975</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
@@ -2653,7 +2656,7 @@
         <v>36.708095989675947</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="L39" s="3" t="s">
         <v>35</v>
@@ -2667,7 +2670,7 @@
         <v>13289.750322558248</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
@@ -2696,7 +2699,7 @@
         <v>38.890872965260115</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>36</v>
@@ -2710,7 +2713,7 @@
         <v>14080</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
@@ -2739,7 +2742,7 @@
         <v>41.203444614108754</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>120</v>
+        <v>209</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>37</v>
@@ -2753,7 +2756,7 @@
         <v>14917.240368578872</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
@@ -2782,7 +2785,7 @@
         <v>43.653528929125486</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="L42" s="3" t="s">
         <v>38</v>
@@ -2796,7 +2799,7 @@
         <v>15804.265640195976</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
@@ -2825,7 +2828,7 @@
         <v>46.249302838954307</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="L43" s="3" t="s">
         <v>39</v>
@@ -2839,7 +2842,7 @@
         <v>16744.036179238312</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -2868,7 +2871,7 @@
         <v>48.99942949771868</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>40</v>
@@ -2882,7 +2885,7 @@
         <v>17739.688382519809</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
@@ -2911,7 +2914,7 @@
         <v>51.913087197493141</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="L45" s="3" t="s">
         <v>41</v>
@@ -2925,7 +2928,7 @@
         <v>18794.545146714081</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
@@ -2954,7 +2957,7 @@
         <v>55</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>42</v>
@@ -2968,7 +2971,7 @@
         <v>19912.126958213179</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -2997,7 +3000,7 @@
         <v>58.270470189761255</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>114</v>
+        <v>211</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>43</v>
@@ -3011,7 +3014,7 @@
         <v>21096.163642423671</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
@@ -3040,7 +3043,7 @@
         <v>61.735412657015516</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>113</v>
+        <v>212</v>
       </c>
       <c r="L48" s="3" t="s">
         <v>44</v>
@@ -3054,7 +3057,7 @@
         <v>22350.606811712249</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -3083,7 +3086,7 @@
         <v>65.406391325149656</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>45</v>
@@ -3097,7 +3100,7 @@
         <v>23679.643053544605</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
@@ -3126,7 +3129,7 @@
         <v>69.295657744218019</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="L50" s="3" t="s">
         <v>46</v>
@@ -3140,7 +3143,7 @@
         <v>25087.707902831939</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -3169,7 +3172,7 @@
         <v>73.416191979351879</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="L51" s="3" t="s">
         <v>47</v>
@@ -3183,7 +3186,7 @@
         <v>26579.500645116499</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
@@ -3212,7 +3215,7 @@
         <v>77.781745930520216</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>48</v>
@@ -3226,7 +3229,7 @@
         <v>28160</v>
       </c>
       <c r="O52" s="3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -3255,7 +3258,7 @@
         <v>82.406889228217494</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="L53" s="3" t="s">
         <v>49</v>
@@ -3269,7 +3272,7 @@
         <v>29834.480737157748</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
@@ -3298,7 +3301,7 @@
         <v>87.307057858250957</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>50</v>
@@ -3312,7 +3315,7 @@
         <v>31608.531280391944</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
@@ -3341,7 +3344,7 @@
         <v>92.498605677908614</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>51</v>
@@ -3355,7 +3358,67 @@
         <v>35479.376765039604</v>
       </c>
       <c r="O55" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J56" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J57" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J58" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J59" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J60" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J61" s="3" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J62" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J63" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J64" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>